<commit_message>
Again on performance optimizations, based on PageSpeed
</commit_message>
<xml_diff>
--- a/SupportFiles/Lighthouse Reports.xlsx
+++ b/SupportFiles/Lighthouse Reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele DM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele DM\source\repos\Michele-traceroute\SupportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16E2AAF-A02D-40C4-9E96-D852A97E2118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F8969C-50AB-4D97-A955-E6FC6267BBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13780" xr2:uid="{DB3C80DA-326C-47D7-8CBE-0265EA689366}"/>
+    <workbookView xWindow="1970" yWindow="1230" windowWidth="19190" windowHeight="9870" xr2:uid="{DB3C80DA-326C-47D7-8CBE-0265EA689366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,12 +137,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{6281D9D3-A093-4D07-9E50-EA9C8537FBE2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michele Di Maria:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+First Contentful Paint</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{9AE60A3D-2532-4CA6-9E44-B2CDC0A95FF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michele Di Maria:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Largest Contentful Paint</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{800D49EF-351E-482E-B564-7321C466A99E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michele Di Maria:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Total Blocking Time</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{0B9328B7-4762-42CF-8A39-0755DB21F1E2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michele Di Maria:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Cumulative Layout Shift</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>Performance</t>
   </si>
@@ -202,7 +298,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,16 +327,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -248,14 +357,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5359B915-CD07-41C9-A1F0-D439A7D39A0F}">
-  <dimension ref="B2:M8"/>
+  <dimension ref="B2:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,7 +895,7 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D7">
         <v>100</v>
@@ -808,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="D8">
         <v>100</v>
@@ -833,11 +952,111 @@
       </c>
       <c r="M8">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B10" s="2">
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>45457</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3">
+        <v>100</v>
+      </c>
+      <c r="E12" s="3">
+        <v>96</v>
+      </c>
+      <c r="F12" s="3">
+        <v>100</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>60</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="M12" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>84</v>
+      </c>
+      <c r="I13">
+        <v>1.2</v>
+      </c>
+      <c r="J13">
+        <v>3.7</v>
+      </c>
+      <c r="K13">
+        <v>180</v>
+      </c>
+      <c r="L13">
+        <v>0.113</v>
+      </c>
+      <c r="M13">
+        <v>2.1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C8">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -850,7 +1069,49 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5D0D6F1C-C7EB-482B-B368-840753279CFE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E811019A-0B9D-45E8-957A-C10883A828A7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M4:M8">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1823FEE8-483E-4E75-9D42-CDA3630607BE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -859,7 +1120,21 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{1823FEE8-483E-4E75-9D42-CDA3630607BE}</x14:id>
+          <x14:id>{35B0AE8D-491E-42CD-94EF-A6811248FD60}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M13">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4821255C-2F77-4F1D-8375-EEA348075694}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -887,6 +1162,32 @@
           <xm:sqref>C4:C8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5D0D6F1C-C7EB-482B-B368-840753279CFE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E811019A-0B9D-45E8-957A-C10883A828A7}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1823FEE8-483E-4E75-9D42-CDA3630607BE}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
@@ -899,6 +1200,32 @@
           </x14:cfRule>
           <xm:sqref>M4:M8</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{35B0AE8D-491E-42CD-94EF-A6811248FD60}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4821255C-2F77-4F1D-8375-EEA348075694}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>M13</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>